<commit_message>
implement daa driven in register page
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/DataDriven.xlsx
+++ b/src/test/resources/testData/DataDriven.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Register" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -20,6 +20,9 @@
     <t>password</t>
   </si>
   <si>
+    <t>error message</t>
+  </si>
+  <si>
     <t>QualityWay</t>
   </si>
   <si>
@@ -32,6 +35,9 @@
     <t>pwd_ds_algo@2Invalid</t>
   </si>
   <si>
+    <t>Invalid Username and Password</t>
+  </si>
+  <si>
     <t>Confirm Password</t>
   </si>
   <si>
@@ -41,19 +47,34 @@
     <t>QualityWayABC</t>
   </si>
   <si>
+    <t>Your password can’t be too similar to your other personal information.</t>
+  </si>
+  <si>
     <t>Quality</t>
   </si>
   <si>
+    <t>Your password must contain at least 8 characters.</t>
+  </si>
+  <si>
     <t>123456789</t>
   </si>
   <si>
+    <t>Your password can’t be entirely numeric.</t>
+  </si>
+  <si>
     <t>pwd_ds_algo@2ABC</t>
   </si>
   <si>
     <t>pwd_ds_algo@2ABCD</t>
   </si>
   <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
     <t>pwd_ds_algo@2valid</t>
+  </si>
+  <si>
+    <t>User already exists</t>
   </si>
 </sst>
 </file>
@@ -108,16 +129,16 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -347,25 +368,33 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -396,81 +425,102 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3"/>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5"/>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement datadriven in try editor window
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/DataDriven.xlsx
+++ b/src/test/resources/testData/DataDriven.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Register" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="TryEditor" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -75,6 +76,33 @@
   </si>
   <si>
     <t>User already exists</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Invalid code</t>
+  </si>
+  <si>
+    <t>print 'welcome'</t>
+  </si>
+  <si>
+    <t>System.out.println('welcome');</t>
+  </si>
+  <si>
+    <t>System.out.println 'welcome</t>
+  </si>
+  <si>
+    <t>welcome</t>
+  </si>
+  <si>
+    <t>NameError: name 'System' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
   </si>
 </sst>
 </file>
@@ -157,6 +185,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
@@ -526,4 +558,56 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.13"/>
+    <col customWidth="1" min="2" max="2" width="28.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>